<commit_message>
🏩🎹 Checkpoint ./server.js:62737451/13528 ./public/scripts.js:62737451/2
</commit_message>
<xml_diff>
--- a/orders.xlsx
+++ b/orders.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14" count="14">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10" count="10">
   <x:si>
     <x:t>Reference Code</x:t>
   </x:si>
@@ -25,37 +25,28 @@
     <x:t>Pending Amount</x:t>
   </x:si>
   <x:si>
+    <x:t>Delivered Amount</x:t>
+  </x:si>
+  <x:si>
     <x:t>Description</x:t>
   </x:si>
   <x:si>
     <x:t>Status</x:t>
   </x:si>
   <x:si>
-    <x:t>{"t":"s","v":"hehe","s":{"fill":{"fgColor":{"rgb":"orange"}}}}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>{"t":"s","v":"Hatdog","s":{"fill":{"fgColor":{"rgb":"orange"}}}}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>{"t":"n","v":100,"s":{"fill":{"fgColor":{"rgb":"orange"}}}}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>{"t":"s","v":"a","s":{"fill":{"fgColor":{"rgb":"orange"}}}}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>{"t":"s","v":"Pending","s":{"fill":{"fgColor":{"rgb":"orange"}}}}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>{"t":"n","v":10,"s":{"fill":{"fgColor":{"rgb":"orange"}}}}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>{"t":"s","v":"aa","s":{"fill":{"fgColor":{"rgb":"orange"}}}}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>{"t":"s","v":"okay","s":{"fill":{"fgColor":{"rgb":"orange"}}}}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>{"t":"n","v":111,"s":{"fill":{"fgColor":{"rgb":"orange"}}}}</x:t>
+    <x:t>CS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Folder</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Long</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Pending</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Short</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -418,7 +409,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:5">
+    <x:row r="1" spans="1:6">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -434,55 +425,47 @@
       <x:c r="E1" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:5">
+    <x:row r="2" spans="1:6">
       <x:c r="A2" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="n">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="n">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6">
+      <x:c r="A3" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="C2" s="0" t="s">
+      <x:c r="B3" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="E2" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:5">
-      <x:c r="A3" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
+      <x:c r="C3" s="0" t="n">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="n">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:5">
-      <x:c r="A4" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="E4" s="0" t="s">
+      <x:c r="F3" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
🏋🍖 Checkpoint ./public/scripts.js:62737451/61 ./public/index.html:62737451/1330 ./public/styles.css:62737451/383 ./server.js:62737451/2500
</commit_message>
<xml_diff>
--- a/orders.xlsx
+++ b/orders.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10" count="10">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12" count="12">
   <x:si>
     <x:t>Reference Code</x:t>
   </x:si>
@@ -34,19 +34,22 @@
     <x:t>Status</x:t>
   </x:si>
   <x:si>
-    <x:t>CS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Folder</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Long</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Pending</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Short</x:t>
+    <x:t>hehe</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Item 1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Desc 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Completed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Item 111111111111111111111111111111111111111111</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Desc 3</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -437,10 +440,10 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C2" s="0" t="n">
-        <x:v>100</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="D2" s="0" t="n">
-        <x:v>90</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
         <x:v>8</x:v>
@@ -454,16 +457,16 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C3" s="0" t="n">
-        <x:v>100</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="D3" s="0" t="n">
-        <x:v>99</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="E3" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="F3" s="0" t="s">
         <x:v>9</x:v>

</xml_diff>

<commit_message>
🎀📯 Checkpoint ./public/scripts.js:62737451/1319 ./server.js:62737451/3900
</commit_message>
<xml_diff>
--- a/orders.xlsx
+++ b/orders.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12" count="12">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13" count="13">
   <x:si>
     <x:t>Reference Code</x:t>
   </x:si>
@@ -34,22 +34,25 @@
     <x:t>Status</x:t>
   </x:si>
   <x:si>
-    <x:t>hehe</x:t>
+    <x:t>CS101</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Item 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Desc 1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Overlapped</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CS103</x:t>
   </x:si>
   <x:si>
     <x:t>Item 1</x:t>
   </x:si>
   <x:si>
-    <x:t>Desc 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>{"value":"Completed","style":{"font":{"color":"black"},"fill":{"type":"pattern","patternType":"solid","fgColor":"darkgreen"}}}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Item 111111111111111111111111111111111111111111</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Desc 3</x:t>
+    <x:t>Completed</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -440,10 +443,10 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C2" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="D2" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>999</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
         <x:v>8</x:v>
@@ -454,22 +457,22 @@
     </x:row>
     <x:row r="3" spans="1:6">
       <x:c r="A3" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C3" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="D3" s="0" t="n">
-        <x:v>4</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="E3" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="F3" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>